<commit_message>
debug and new bar of reg and get timeline
</commit_message>
<xml_diff>
--- a/admission54.xlsx
+++ b/admission54.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thirapat\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khunach\Desktop\projectkmitl\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -204,7 +204,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -220,7 +220,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ธีมของ Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -484,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -680,7 +680,7 @@
         <v>26</v>
       </c>
       <c r="B8">
-        <v>270</v>
+        <v>279</v>
       </c>
       <c r="C8">
         <v>15</v>

</xml_diff>